<commit_message>
updated DPP upload code
</commit_message>
<xml_diff>
--- a/db_feed/DPPDTT/DPPDTT_dataset_feed_D6_ALcopy.xlsx
+++ b/db_feed/DPPDTT/DPPDTT_dataset_feed_D6_ALcopy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\db_feed\DPPDTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliu319\Documents\GitHub\ofet-db\db_feed\DPPDTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B5B6A-01D9-4D23-95D8-34F819A33BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9783BFBD-E407-46B2-AEE6-C1C6909207AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPPDTT_D6_combined (raw)" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="polymer" sheetId="6" r:id="rId8"/>
     <sheet name="solution_makeup_polymer" sheetId="13" r:id="rId9"/>
     <sheet name="solution_treatment" sheetId="14" r:id="rId10"/>
-    <sheet name="solution_treatment_order" sheetId="23" r:id="rId11"/>
-    <sheet name="solution_treatment_step" sheetId="24" r:id="rId12"/>
+    <sheet name="solution_treatment_step" sheetId="24" r:id="rId11"/>
+    <sheet name="solution_treatment_order" sheetId="23" r:id="rId12"/>
     <sheet name="device_fabrication" sheetId="15" r:id="rId13"/>
     <sheet name="substrate_pretreat" sheetId="16" r:id="rId14"/>
     <sheet name="substrate_pretreat_step" sheetId="18" r:id="rId15"/>
@@ -24919,8 +24919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2B1B37-3478-4ED9-8C8E-E87200A72E2D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24945,48 +24945,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D0F74D-EB4A-49BC-9FAF-46A05638A96A}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F1F663-9F56-4E39-9F36-D3287E533545}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -25034,6 +24992,48 @@
       </c>
       <c r="E2" s="24">
         <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D0F74D-EB4A-49BC-9FAF-46A05638A96A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -27748,7 +27748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE0F98E-1558-4CEC-B9BF-15230FA6A859}">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>

</xml_diff>